<commit_message>
fixing ClassCastException in the integration tests
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it-graph/src/test/resources/standard_excel_files/Indirect_Fx.xlsx
+++ b/calculation-engine/engine-tests/engine-it-graph/src/test/resources/standard_excel_files/Indirect_Fx.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\SpreadSheet\master\calculation-engine\engine-demo\src\main\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spreadsheet\CalculationEngine\calculation-engine\engine-tests\engine-it-graph\src\test\resources\standard_excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -357,7 +357,7 @@
   <dimension ref="A2:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,20 +396,20 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6">
-        <f ca="1">INDIRECT(A2)</f>
-        <v>1.333</v>
+        <f>2+3</f>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7">
-        <f ca="1">INDIRECT("Bolt")</f>
-        <v>10</v>
+        <f>3+6</f>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <f ca="1">INDIRECT("B"&amp;A5)</f>
-        <v>62</v>
+      <c r="C8" t="b">
+        <f>1=8</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -427,6 +427,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000BBA6CFB0E2DE4B9D0F8FC00657BC00" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b5fa52e5d42efb553dd3c6ab2e94e30b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -540,20 +546,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4ACC23D-618F-498F-82B7-E879AABF45F4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4ACC23D-618F-498F-82B7-E879AABF45F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F48C0B06-AFE3-40CA-8DC7-5A3B093035C3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24ED49B9-6DDA-48A7-955F-280F858B545A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24ED49B9-6DDA-48A7-955F-280F858B545A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F48C0B06-AFE3-40CA-8DC7-5A3B093035C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>